<commit_message>
ready for user test
</commit_message>
<xml_diff>
--- a/tasks1.xlsx
+++ b/tasks1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E44BD1-09F1-4F98-BFF9-E16884DF976A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB08429-194A-48C2-AB70-F271A3956CBB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="107">
   <si>
     <t>hint_2</t>
   </si>
@@ -329,12 +329,6 @@
 &amp;nbsp;&amp;nbsp;createCanvas(width, height);&lt;br&gt;
 }
 </t>
-  </si>
-  <si>
-    <t>if(&lt;b style="color:#36047c"&gt;false,/b&gt;){ &lt;br&gt;
-&amp;nbsp;&amp;nbsp;x += random(-1, 1);&lt;br&gt;
-&amp;nbsp;&amp;nbsp;y += random(-1, 1);&lt;br&gt;
-}</t>
   </si>
   <si>
     <t>mouseX &lt;br&gt;</t>
@@ -450,6 +444,21 @@
   </si>
   <si>
     <t>rotate(a)</t>
+  </si>
+  <si>
+    <t>Final Test</t>
+  </si>
+  <si>
+    <t>if(&lt;b style="color:#36047c"&gt;false&lt;/b&gt;){ &lt;br&gt;
+&amp;nbsp;&amp;nbsp;x += random(-1, 1);&lt;br&gt;
+&amp;nbsp;&amp;nbsp;y += random(-1, 1);&lt;br&gt;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congratulations on your completion on all the tutorials!&lt;br&gt;
+Now Let's use all we've learned to create a interesting interaction effect!
+&lt;a href="test.html" target="_blank"&gt;Click herel&lt;/a&gt; to preview the final effects!
+</t>
   </si>
 </sst>
 </file>
@@ -789,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1183,10 +1192,10 @@
         <v>2</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="180">
@@ -1197,22 +1206,22 @@
         <v>3</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="120">
@@ -1223,119 +1232,130 @@
         <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="135">
       <c r="A20" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="K20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="165">
       <c r="A21" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="3">
         <v>2</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="105">
       <c r="A22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B22" s="3">
         <v>3</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="409.5">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3">
         <v>4</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="150">
       <c r="A24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="3">
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:11" ht="180">
+      <c r="A25" s="2" t="s">
         <v>104</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>